<commit_message>
updated after classification was complete
</commit_message>
<xml_diff>
--- a/Volunteers_2022/Volunteer Reports Being Coded/CleoRandall_CoyoteReports.xlsx
+++ b/Volunteers_2022/Volunteer Reports Being Coded/CleoRandall_CoyoteReports.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Farr\Github\EdmontonUrbanCoyotes\Volunteers_2022\Volunteer Reports Being Coded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FB23F6-E51D-4654-9965-26A6DC4BC39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB10CC7-3E26-4954-8727-87FB36839763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{05804418-2EB1-4633-9D5C-4566DCE76D51}"/>
+    <workbookView xWindow="-25320" yWindow="225" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{05804418-2EB1-4633-9D5C-4566DCE76D51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="336">
   <si>
     <t>sighting</t>
   </si>
@@ -721,6 +722,347 @@
   </si>
   <si>
     <t>One coyote, headed south.</t>
+  </si>
+  <si>
+    <t>Between terwillegar drive and Turvey Bend/ edge terwillegar town/lake/service road</t>
+  </si>
+  <si>
+    <t>Walking my dog on leash briefly down path and entered dip through woods to access service road by terwillegar town.  My dog quickened his pace through dip, pulling me in a hurry.  Once on service road there was a smallish coyote arched back, tail between legs and hissing. I yelled NO at it and picked up some gravel and threw it at it.  It trotted into the woods where I just came from.  Then I noticed another larger one to my left (not as close) coming towards me slowly.  I yelled NO and threw gravel again.  Not sure if I should continue down road as unsure how many and if the one on my left would follow me.  Went back through dip in woods quickly and looked back to see coyote in grass/path where I just went through. Apparently there are signs on one end of this path/road but not where I entered on the side street by Turvey Bend.  I spoke to locals who confirmed there must be a den 100 yards in from the access point.  Maybe some extra signs on both ends warning of active den and not to walk there would be good.  I like coyotes generally and never have issues normally but clearly I was in the wrong place.</t>
+  </si>
+  <si>
+    <t>53 ave 174 Street</t>
+  </si>
+  <si>
+    <t>solo coyote sniffing light standard base, returned to ravine</t>
+  </si>
+  <si>
+    <t>23 rd avenue and saddleback road</t>
+  </si>
+  <si>
+    <t>lone female coyote came out of crescent across from St. Therese school.  She has a litter of 6 pups in that crescent.  She has been in the school yard several days now, suntanning? Crows are dive bombing her and she is jumping at them.  Apparently she approach and couple of kids walking their dog as well.  They ran to a truck in the area of help.  The guy in the truck then warned me as did several others.   She apparently went into the valley just north of the saddleback walkway.</t>
+  </si>
+  <si>
+    <t>Ellerslie Rd and Rutherford Gate</t>
+  </si>
+  <si>
+    <t>It was trying to cross the road</t>
+  </si>
+  <si>
+    <t>Rutherford road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 full grown coyotes, walking awar from 3 different people out walking their dogs, who clearly had just encountered these coyotes. I was driving and saw them walking before I saw the people who I mentioned previously. </t>
+  </si>
+  <si>
+    <t>112 Street NW and 25 Avenue NW</t>
+  </si>
+  <si>
+    <t>Coyote was initially crossing road (from park into neighbourhood). I honked the car horn. The coyote ran a short distance and stopped by the community mailbox. I honked again; however, the coyote did not move. As my house was near, I parked the car, exited, and then ran towards the coyote. It ran from me into Blue Quill Park (open space on map), then lay down, very comfortably. By then, a large crow was also following it quite closely._x000D_
+I am not concerned for my own children as they are not small, but there are quite a few small children in this community.</t>
+  </si>
+  <si>
+    <t>I noticed what at first I thought was a dog on my neighbour&amp;#039;s yard, then realized it had a bushy tail and suspected that it was a coyote. I was either coming or leaving home, entering or exiting my car in the house to the north of the location pin, and the coyote seemed very comfortable, it did not try to run even when I attempted to take a photo (because I was still not sure what it was). After trying to take a photo, I did take one or two running steps towards it, at which point it left the neighbour&amp;#039;s yard.</t>
+  </si>
+  <si>
+    <t>147 street x 109 ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A medium sized coyote trotted south from 109 Ave to 147 street then turned east into the alley. It did not seem distressed or injured or chasing anything or being chased. It was notable simple because it was almost 10am on a Saturday and I was surprised to see it out and about. </t>
+  </si>
+  <si>
+    <t>James Mowatt trail and Bowen Wynd</t>
+  </si>
+  <si>
+    <t>Full grown coyote hanging out in the field where children play</t>
+  </si>
+  <si>
+    <t>13/06/2021</t>
+  </si>
+  <si>
+    <t>111 st and 23 ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He was around the sobeys trying to cross and get back to the ravine. _x000D_
+He looked a little thin but fine. Just kind of chilling and trying to cross the street. We were driving past. </t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I followed 2 smallish coyotes (only because we were headed the same way) along trail that goes around south parking lot in Rainbow valley. Probably for close to a minute, with the coyotes pausing, one taking a pee break, as they eyed me warily.  They left the trail just out of my sight around a bend. _x000D_
+</t>
+  </si>
+  <si>
+    <t>14/06/2021</t>
+  </si>
+  <si>
+    <t>167C Ave McConachie  Way NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heading South on McConachie Way. Saw a rabbit and bolted West down 167C Ave. More than likely the same coyote reported around our area last year. </t>
+  </si>
+  <si>
+    <t>58 ave, riverbend rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looked big and healthy. Alone. It was walking along the path. </t>
+  </si>
+  <si>
+    <t>Ellerslie Road and 111st</t>
+  </si>
+  <si>
+    <t>Ran across the road into a apartment complex.  I have been seeing quite a few coyotes in my neighborhood.  Coming down walking baths and up streets.  This is a concern when I&amp;rsquo;m out for a walk with my kids and one follows us down a path or street.  I have lived in the MacEwan neighborhood for almost 18 years and this is the worst I have ever seen.  I like seeming them in the fields behind my house but when they are following my kids and wife through the streets that is no longer ok.</t>
+  </si>
+  <si>
+    <t>Ellerslie Road and 111 St</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A very healthy adult carrying a healthy pup in its mouth. It was running on the green space along the laneway behind the Save On Foods, crossed in front of the Condo parking entrance and went behind a fence. My guess is it was moving it&amp;#039;s pups. Pup was still all gray in colour and about the size of a teddy bear. It was in no way concerned about cars driving nearby, and determined on where it was going. </t>
+  </si>
+  <si>
+    <t>15/06/2021</t>
+  </si>
+  <si>
+    <t>101A Ave between 57 &amp;amp; 52 Street</t>
+  </si>
+  <si>
+    <t>4 coyote followed me and my dog for several blocks. We were on the n side of 101A Ave, the coyotes remained on the south side of the Ave tracking us from 57 to 52 St. They disappeared into the copse of trees on the west side of the 50 St / 101 Ave electrical substation.</t>
+  </si>
+  <si>
+    <t>16/06/2021</t>
+  </si>
+  <si>
+    <t>Tomlinson Common NW &amp;amp; Thibault Way NW</t>
+  </si>
+  <si>
+    <t>Coyote was sitting alone on the edge of the tree line. I believe this is the same coyote I sighted the last two times I visited this area. We immediately backed out of the area. Minutes later we noticed that it had walked south along the tree line. Then walked east towards the late. It looked fine.</t>
+  </si>
+  <si>
+    <t>17/06/2021</t>
+  </si>
+  <si>
+    <t>Blue Quill Community League hill facing 25 Ave and 112 st</t>
+  </si>
+  <si>
+    <t>Two coyotes sleeping on the hill. They have been charging at dogs when people are walking past on the sidewalk on the mornings of June 16 &amp;amp; 17 (reported on community league forum).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 Ave 115 St </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A coyote charged my dog in front of our house, and chased her into our backyard where I was doing yard work. It ran off when it saw me. </t>
+  </si>
+  <si>
+    <t>27 Ave 117 st nw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The coyote was wandering up and down the residential streets and had ripped open all.the garbage bags as it was collections day.  He was not at all intimidated by humans </t>
+  </si>
+  <si>
+    <t>Saddleback Road and 112 Street NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Came very close to townhouse gates, moving quite quickly </t>
+  </si>
+  <si>
+    <t>25 Ave, 113 Street</t>
+  </si>
+  <si>
+    <t>Aggressive coyote charged at human and dog snarling and growling - yelling, rock throwing and kicking only made it back off slightly - it did NOT run away</t>
+  </si>
+  <si>
+    <t>Blue quill community field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laying 5 feet from main sidewalk._x000D_
+Pulled over vehicle to yell/honk at it to get it to move away - opened eyes but wouldn&amp;rsquo;t even lift its head. No fear or desire to move. </t>
+  </si>
+  <si>
+    <t>What3words location: trail.brief.explorer</t>
+  </si>
+  <si>
+    <t>Large grey, white, orange coyote. Healthy tail, but appeared to be limping. Looked at me about 150m away and walked into trees and underbrush out of view.</t>
+  </si>
+  <si>
+    <t>18/06/2021</t>
+  </si>
+  <si>
+    <t>wolf willow ravine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single coyote followed and crossed walking path </t>
+  </si>
+  <si>
+    <t>19/06/2021</t>
+  </si>
+  <si>
+    <t>127 Street &amp;amp; Villa Avenue</t>
+  </si>
+  <si>
+    <t>Was walking my dog.  Encountered 3 coyotes (seemed adult) as I rounded the corner heading North.  2 coyotes approached, one hung back.  Made myself large-ish, made noise, one lunged toward me before I picked up my dog and backed away.  Fortunately a car came down the street and they backed off a bit further. I&amp;#039;ve had a few encounters previously; this felt the most potentially risky.</t>
+  </si>
+  <si>
+    <t>111 st / saddleback road</t>
+  </si>
+  <si>
+    <t>129th avenue and fort road</t>
+  </si>
+  <si>
+    <t>Skinny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">122 Street 41 Avenue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coyote Took my friends cat by the head _x000D_
+She chased the coyote and attacked it and coyote dropped cat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">122 street and 111 avenue in park on north side of Ave </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I was walking my 7lb dog on leash and turned one way to see if anyone was coming down bike lane, turned other way and coyote was going back and forth side to side seeing how to get to my dog, it was only like 4 metres away. I grabbed dog, screamed at coyote, tried to scare it waving arms and yelling and it just stood and stared at me. Then I left and it went on the hill by the playground and stared at us </t>
+  </si>
+  <si>
+    <t>40street and 168A avenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walked along 40 street and as I saw it I followed it as it was heading to a local park which I thought my kids were at and shooed it away towards Manning drive. </t>
+  </si>
+  <si>
+    <t>20/06/2021</t>
+  </si>
+  <si>
+    <t>103 Avenue 137 Street</t>
+  </si>
+  <si>
+    <t>Calmly walking through the neighborhood. He/She followed us for about 10 metres and then wandered away. I did take photos</t>
+  </si>
+  <si>
+    <t>St. George&amp;rsquo;s Crescent &amp;amp; 102 Ave</t>
+  </si>
+  <si>
+    <t>Two coyotes in ravine bush by St George&amp;rsquo;s Crescent trailing us as we walked our dog</t>
+  </si>
+  <si>
+    <t>St Georges Crescent and 135 St - green space above MacKinnon Ravine</t>
+  </si>
+  <si>
+    <t>two sightings in same green space.  June 11 at 9:30 am and June 18 at about same time.  single coyote.  healthy looking.  came out when the dog was sniffing at the periphery.  no engagement but was close and kept an eye until we moved off</t>
+  </si>
+  <si>
+    <t>St. Georges Cres and Stony Plain Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">One coyote approached me and my dog coming from the southeast side  of St. George Cres. I yelled and threw a stick at her and she jumped into the ravine on the east side the cres, emerging moments later with a second coyote. Both escorted us south on St. Georges until I threw more sticks. they jumoped back into the ravine and did not reapper. </t>
+  </si>
+  <si>
+    <t>22/06/2021</t>
+  </si>
+  <si>
+    <t>Callaghan Drive SW, north end of stormwater pond.</t>
+  </si>
+  <si>
+    <t>A lone coyote was looking for prey, moving in and out of the tall grasses/bushes on the northwest side of the Callaghan stormwater pond. A lone male was walking northbound on the walking path and the coyote fled eastwards towards Blackmud Creek once he noticed the person.</t>
+  </si>
+  <si>
+    <t>23/06/2021</t>
+  </si>
+  <si>
+    <t>79 St NW and 124 Ave</t>
+  </si>
+  <si>
+    <t>Walking coyote in the front of the house&amp;#039;s. The Magpies scream wake me up.</t>
+  </si>
+  <si>
+    <t>25/06/2021</t>
+  </si>
+  <si>
+    <t>72 avenue nw and 111 street nw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back yard </t>
+  </si>
+  <si>
+    <t>26/06/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the second time this coyote come. It&amp;#039;s right under my bedroom window. I think it smells my cat. </t>
+  </si>
+  <si>
+    <t>Blackmore Court and Blackmud Creek Crescent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This morning I heard two magpies making noise outside, looked up and saw a healthy looking lone coyote in my front yard that was just going yard to yard sniffing. I have never seen a coyote so close before and was just very surprised.  </t>
+  </si>
+  <si>
+    <t>75 street 152C Ave</t>
+  </si>
+  <si>
+    <t>walked from SE down middle of street, circled several parked cars. chased rabbit from neighbor&amp;rsquo;s driveway back to area it came from.</t>
+  </si>
+  <si>
+    <t>27/06/2021</t>
+  </si>
+  <si>
+    <t>111th and Elersile</t>
+  </si>
+  <si>
+    <t>Seen by east side of the intersection, going between side walks, clearly panting (possibly due to heat exhaustion)</t>
+  </si>
+  <si>
+    <t>Near Rutherford</t>
+  </si>
+  <si>
+    <t>It was alone and it was standing there but then left when it looked at us</t>
+  </si>
+  <si>
+    <t>111 street Ellerslie Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Looked very overheated, alone, shaggy looking, jaunt pace running on the grass </t>
+  </si>
+  <si>
+    <t>28/06/2021</t>
+  </si>
+  <si>
+    <t>west of Rabbit Hill Rd, on utility corridor path</t>
+  </si>
+  <si>
+    <t>lone coyote; appeared young; sandy colour coat; looked at me then started running east on grassy surface next to the path</t>
+  </si>
+  <si>
+    <t>134 St NW &amp;amp; 153 Ave</t>
+  </si>
+  <si>
+    <t>Lone coyote walking in the long grass on the mixed use pathway between the townhomes along 153rd and the houses in Skyview/Cumberland, headed East, just going about it&amp;#039;s business. My dog and I were quite close, but no interaction.</t>
+  </si>
+  <si>
+    <t>100 avenue 140 street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My cat and I were cooling off in the backyard with the gate open and she went from sleeping to a top speed run in a second. I ran after her thinking it was a cat but she was chasing a coyote who tried to enter her yard. I yelled at him as he was running away. Because of the heat we stayed out, with the gate closed and an hour later he was back. He was on my driveway two feet from the back gate. I put the cat in the house, grabbed a handful of gravel and chased him away a second time. They&amp;#039;re getting braver and less fearful over the 20 years I&amp;#039;ve been here. I&amp;#039;m sitting outside now with a shovel for protection. I&amp;#039;m wondering how many other cats are as brave/foolish as mine to aggress against a coyote. </t>
+  </si>
+  <si>
+    <t>29/06/2021</t>
+  </si>
+  <si>
+    <t>S. Terwillegar blvd NW &amp;amp; Southesk Landing</t>
+  </si>
+  <si>
+    <t>Around 4am, I had the screen door open and heard a thump. Looked up to see that a coyote had chased a cat onto my front porch. It grabbed the cornered cat and headed toward park. The cat fought back, got away and they bolted east down S. Terwillegar and I lost sight of them.</t>
+  </si>
+  <si>
+    <t>30/06/2021</t>
+  </si>
+  <si>
+    <t>3:30am, noticed a coyote patrolling the park. It didn&amp;#039;t cross the street into the residential area. It headed west toward the pond before I lost sight.</t>
+  </si>
+  <si>
+    <t>Blackmud Creek Drive and Blackmud Creek Crescent</t>
+  </si>
+  <si>
+    <t>Coyote was running along sidewalk at 4.15 pm. He was heading south then towards the west towards the Roberta MacAdams school yard. Very concerning that this is such a public area in the middle of the day when children would normally be walking home from school.</t>
   </si>
 </sst>
 </file>
@@ -982,50 +1324,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1256,16 +1554,60 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thick">
           <color theme="0"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color theme="0"/>
-        </bottom>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1282,18 +1624,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6044FA7-8662-458E-9F72-7D1A6BAD62B7}" name="Table1" displayName="Table1" ref="A1:I101" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6044FA7-8662-458E-9F72-7D1A6BAD62B7}" name="Table1" displayName="Table1" ref="A1:I101" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:I101" xr:uid="{F6044FA7-8662-458E-9F72-7D1A6BAD62B7}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{D61422D3-B0C7-4B57-A8A1-85DEC6C90950}" name="ID" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{E024FA86-6AAF-4FCA-BD98-C5F711501C63}" name="Date" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{D493B7AA-2FE7-48F4-B135-E711BC6352EF}" name="Lat" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{97A072BB-B87F-4FAD-9522-D47A69B75222}" name="Long" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{62816C07-8705-458B-A8F0-247068BE0939}" name="Time" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{69E5BCD6-95CA-40C0-BFEB-F45BA6FD23C3}" name="Date2" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{D5537CDE-234A-4C79-BD24-98EB1DEED80C}" name="Type" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{AEBEE45A-D089-4C88-9DC7-0969D08F6D95}" name="Location" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{B5EE9E51-F467-408F-81EA-119E5FFF0C7C}" name="Comments" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{D61422D3-B0C7-4B57-A8A1-85DEC6C90950}" name="ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{E024FA86-6AAF-4FCA-BD98-C5F711501C63}" name="Date" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{D493B7AA-2FE7-48F4-B135-E711BC6352EF}" name="Lat" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{97A072BB-B87F-4FAD-9522-D47A69B75222}" name="Long" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{62816C07-8705-458B-A8F0-247068BE0939}" name="Time" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{69E5BCD6-95CA-40C0-BFEB-F45BA6FD23C3}" name="Date2" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{D5537CDE-234A-4C79-BD24-98EB1DEED80C}" name="Type" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{AEBEE45A-D089-4C88-9DC7-0969D08F6D95}" name="Location" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{B5EE9E51-F467-408F-81EA-119E5FFF0C7C}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1598,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D3B5E8-C0D8-4F62-9993-89682E6C6BCB}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4303,4 +4645,1340 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDBF6E7F-B502-4B82-BA56-4E577D5106C5}">
+  <dimension ref="A1:I51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="24.88671875" style="16" customWidth="1"/>
+    <col min="9" max="9" width="66.5546875" style="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="257.39999999999998" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>10569</v>
+      </c>
+      <c r="B2" s="8">
+        <v>44356.724999999999</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F2" s="11">
+        <v>44445</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>10570</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44356.749305555553</v>
+      </c>
+      <c r="C3" s="3">
+        <v>53.490570320000003</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-113.6242385</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F3" s="5">
+        <v>44445</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>10571</v>
+      </c>
+      <c r="B4" s="8">
+        <v>44357.518055555556</v>
+      </c>
+      <c r="C4" s="9">
+        <v>53.441238009999999</v>
+      </c>
+      <c r="D4" s="9">
+        <v>-113.5282368</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F4" s="11">
+        <v>44475</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>10572</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44357.681250000001</v>
+      </c>
+      <c r="C5" s="3">
+        <v>53.424798209999999</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-113.52424569999999</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="5">
+        <v>44445</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>10573</v>
+      </c>
+      <c r="B6" s="8">
+        <v>44358.493750000001</v>
+      </c>
+      <c r="C6" s="9">
+        <v>53.422064730000002</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-113.5343469</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F6" s="11">
+        <v>44383</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>10574</v>
+      </c>
+      <c r="B7" s="2">
+        <v>44358.50277777778</v>
+      </c>
+      <c r="C7" s="3">
+        <v>53.457881159999999</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-113.5216064</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F7" s="5">
+        <v>44506</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>10575</v>
+      </c>
+      <c r="B8" s="8">
+        <v>44358.508333333331</v>
+      </c>
+      <c r="C8" s="9">
+        <v>53.457277619999999</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-113.52090099999999</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F8" s="11">
+        <v>44414</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>10576</v>
+      </c>
+      <c r="B9" s="2">
+        <v>44359.508333333331</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="5">
+        <v>44536</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>10577</v>
+      </c>
+      <c r="B10" s="8">
+        <v>44359.839583333334</v>
+      </c>
+      <c r="C10" s="9">
+        <v>53.41680427</v>
+      </c>
+      <c r="D10" s="9">
+        <v>-113.519053</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="F10" s="11">
+        <v>44536</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10578</v>
+      </c>
+      <c r="B11" s="2">
+        <v>44360.660416666666</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>10579</v>
+      </c>
+      <c r="B12" s="8">
+        <v>44360.854166666664</v>
+      </c>
+      <c r="C12" s="9">
+        <v>53.480880339999999</v>
+      </c>
+      <c r="D12" s="9">
+        <v>-113.5539928</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>10580</v>
+      </c>
+      <c r="B13" s="2">
+        <v>44361.466666666667</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>10581</v>
+      </c>
+      <c r="B14" s="8">
+        <v>44361.473611111112</v>
+      </c>
+      <c r="C14" s="9">
+        <v>53.494680879999997</v>
+      </c>
+      <c r="D14" s="9">
+        <v>-113.5802824</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="F14" s="11">
+        <v>44506</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>10582</v>
+      </c>
+      <c r="B15" s="2">
+        <v>44361.788194444445</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>10583</v>
+      </c>
+      <c r="B16" s="8">
+        <v>44361.81527777778</v>
+      </c>
+      <c r="C16" s="9">
+        <v>53.425487109999999</v>
+      </c>
+      <c r="D16" s="9">
+        <v>-113.5203243</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>10584</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44363.03402777778</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>10585</v>
+      </c>
+      <c r="B18" s="8">
+        <v>44363.952777777777</v>
+      </c>
+      <c r="C18" s="9">
+        <v>53.447225260000003</v>
+      </c>
+      <c r="D18" s="9">
+        <v>-113.58963799999999</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>10586</v>
+      </c>
+      <c r="B19" s="2">
+        <v>44364.611805555556</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>10587</v>
+      </c>
+      <c r="B20" s="8">
+        <v>44364.613888888889</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F20" s="11">
+        <v>44322</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>10588</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44364.623611111114</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>10589</v>
+      </c>
+      <c r="B22" s="8">
+        <v>44364.630555555559</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>10590</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44364.644444444442</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>10591</v>
+      </c>
+      <c r="B24" s="8">
+        <v>44364.645833333336</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>10592</v>
+      </c>
+      <c r="B25" s="2">
+        <v>44364.748611111114</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>10593</v>
+      </c>
+      <c r="B26" s="8">
+        <v>44365.470138888886</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>10594</v>
+      </c>
+      <c r="B27" s="2">
+        <v>44366.0625</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>10595</v>
+      </c>
+      <c r="B28" s="8">
+        <v>44366.564583333333</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="I28" s="12"/>
+    </row>
+    <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>10596</v>
+      </c>
+      <c r="B29" s="2">
+        <v>44366.636805555558</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>10597</v>
+      </c>
+      <c r="B30" s="8">
+        <v>44366.79791666667</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>10598</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44366.804166666669</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="5">
+        <v>44142</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>10599</v>
+      </c>
+      <c r="B32" s="8">
+        <v>44366.984027777777</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>10600</v>
+      </c>
+      <c r="B33" s="2">
+        <v>44367.669444444444</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>10601</v>
+      </c>
+      <c r="B34" s="8">
+        <v>44368.013888888891</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>10602</v>
+      </c>
+      <c r="B35" s="2">
+        <v>44368.020833333336</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="F35" s="5">
+        <v>44506</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>10603</v>
+      </c>
+      <c r="B36" s="8">
+        <v>44368.6</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>10604</v>
+      </c>
+      <c r="B37" s="2">
+        <v>44369.683333333334</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>10605</v>
+      </c>
+      <c r="B38" s="8">
+        <v>44370.297222222223</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>10608</v>
+      </c>
+      <c r="B39" s="2">
+        <v>44372.6</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
+        <v>10609</v>
+      </c>
+      <c r="B40" s="8">
+        <v>44373.336805555555</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>10610</v>
+      </c>
+      <c r="B41" s="2">
+        <v>44373.374305555553</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
+        <v>10611</v>
+      </c>
+      <c r="B42" s="8">
+        <v>44373.469444444447</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>10612</v>
+      </c>
+      <c r="B43" s="2">
+        <v>44374.49722222222</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>10613</v>
+      </c>
+      <c r="B44" s="8">
+        <v>44374.909722222219</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F44" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H44" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="I44" s="12" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>10614</v>
+      </c>
+      <c r="B45" s="2">
+        <v>44374.999305555553</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
+        <v>10615</v>
+      </c>
+      <c r="B46" s="8">
+        <v>44375.481944444444</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="I46" s="12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>10616</v>
+      </c>
+      <c r="B47" s="2">
+        <v>44375.497916666667</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="4">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
+        <v>10618</v>
+      </c>
+      <c r="B48" s="8">
+        <v>44377.084027777775</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>10619</v>
+      </c>
+      <c r="B49" s="2">
+        <v>44377.244444444441</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
+        <v>10620</v>
+      </c>
+      <c r="B50" s="8">
+        <v>44377.24722222222</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>10621</v>
+      </c>
+      <c r="B51" s="2">
+        <v>44377.979166666664</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>